<commit_message>
Attempt to fix conflict with tables
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlo\Documents\Trabajo\BPI Challenge\bpi-challenge-performance-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5874AC3B-B099-4E1F-9050-A445EC845A39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59BDC2D6-4F1C-4819-A6C1-2F519C9D3A3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17055" yWindow="3270" windowWidth="22800" windowHeight="9975" firstSheet="1" activeTab="2" xr2:uid="{5092433A-F3BB-4CC2-93C1-BDF3BEBCFA24}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{5092433A-F3BB-4CC2-93C1-BDF3BEBCFA24}"/>
   </bookViews>
   <sheets>
     <sheet name="BPI challenge similarity" sheetId="1" r:id="rId1"/>
     <sheet name="Frequent operations" sheetId="2" r:id="rId2"/>
     <sheet name="Question similarity" sheetId="3" r:id="rId3"/>
+    <sheet name="Hoja1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="133">
   <si>
     <t>BPI</t>
   </si>
@@ -266,41 +267,182 @@
     <t>Question - Question</t>
   </si>
   <si>
-    <t>Q1 2017 - Q1 2017</t>
-  </si>
-  <si>
-    <t>Q2 2020 - Q2 2020</t>
-  </si>
-  <si>
-    <t>Q5 2020 - Q5 2020</t>
-  </si>
-  <si>
-    <t>Q2 2019 - Q2 2019</t>
-  </si>
-  <si>
-    <t>Q5 2020 - Q6 2020</t>
-  </si>
-  <si>
-    <t>Q5 2015 - Q5 2015</t>
-  </si>
-  <si>
-    <t>Q6 2020 - Q6 2020</t>
-  </si>
-  <si>
-    <t>Q1 2020 - Q1 2020</t>
-  </si>
-  <si>
-    <t>Q2 2019 - Q1 2020</t>
-  </si>
-  <si>
-    <t>Q4 2020 - Q6 2020</t>
+    <t>Similarity per questions using the Sørensen–Dice coefficient  (AVG: average, STD: standard deviation, VAR:Variance)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q1 2017 - Q1 2017 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q2 2020 - Q2 2020 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q5 2020 - Q5 2020 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q2 2019 - Q2 2019 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q5 2020 - Q6 2020 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q5 2015 - Q5 2015 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q6 2020 - Q6 2020 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q1 2020 - Q1 2020 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q2 2019 - Q1 2020 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q4 2020 - Q6 2020 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q1 2017 - Q5 2020 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q4 2020 - Q5 2020 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q5 2015 - Q1 2017 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q5 2015 - Q2 2019 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q1 2017 - Q2 2019 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q1 2017 - Q6 2020 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q5 2015 - Q1 2020 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q5 2015 - Q2 2020 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q5 2015 - Q5 2020 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q1 2017 - Q1 2020 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q1 2020 - Q2 2020 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q4 2020 - Q4 2020 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q5 2015 - Q6 2020 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q1 2020 - Q4 2020 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q2 2019 - Q4 2020 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q2 2020 - Q5 2020 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q1 2017 - Q4 2020 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q2 2019 - Q2 2020 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q2 2019 - Q5 2020 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q1 2020 - Q6 2020 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q2 2019 - Q6 2020 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q2 2020 - Q6 2020 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q5 2015 - Q4 2020 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q1 2020 - Q5 2020 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q1 2017 - Q2 2020 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q2 2020 - Q4 2020 </t>
+  </si>
+  <si>
+    <t>Distribution of reports and answers of participants per year</t>
+  </si>
+  <si>
+    <t>Reports , Answers</t>
+  </si>
+  <si>
+    <t>Participant</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>2 , 2</t>
+  </si>
+  <si>
+    <t>13 , 13</t>
+  </si>
+  <si>
+    <t>5 , 5</t>
+  </si>
+  <si>
+    <t>2 , 10</t>
+  </si>
+  <si>
+    <t>22 , 30</t>
+  </si>
+  <si>
+    <t>Professional</t>
+  </si>
+  <si>
+    <t>3 , 3</t>
+  </si>
+  <si>
+    <t>6 , 6</t>
+  </si>
+  <si>
+    <t>12 , 50</t>
+  </si>
+  <si>
+    <t>26 , 64</t>
+  </si>
+  <si>
+    <t>Academic</t>
+  </si>
+  <si>
+    <t>4 , 4</t>
+  </si>
+  <si>
+    <t>6 , 24</t>
+  </si>
+  <si>
+    <t>14 , 32</t>
+  </si>
+  <si>
+    <t>62 , 126</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -310,6 +452,14 @@
     </font>
     <font>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -342,7 +492,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -375,7 +525,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -700,17 +860,17 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -889,10 +1049,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="11"/>
+      <c r="B1" s="12"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -1040,10 +1200,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1EB05C4-26F0-4C9B-94D5-9C16319513BC}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1054,161 +1214,684 @@
     <col min="4" max="4" width="15.5703125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C2" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D2" s="13" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B2" s="7">
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3">
         <v>0.22</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C3">
         <v>0.02</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D3">
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" s="7">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4">
         <v>0.21</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C4">
         <v>0.09</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D4">
         <v>0.3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="B4" s="7">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5">
         <v>0.2</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C5">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D5">
         <v>0.26</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="B5" s="7">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6">
         <v>0.18</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C6">
         <v>0.01</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D6">
         <v>0.11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="B6" s="7">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7">
         <v>0.18</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C7">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D7">
         <v>0.26</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B7" s="7">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8">
         <v>0.17</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C8">
         <v>0.02</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D8">
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="B8" s="7">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9">
         <v>0.17</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C9">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D9">
         <v>0.26</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="B9" s="7">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10">
         <v>0.16</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C10">
         <v>0.03</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D10">
         <v>0.18</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="B10" s="7">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11">
         <v>0.13</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C11">
         <v>0.01</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D11">
         <v>0.11</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="B11" s="7">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12">
         <v>0.13</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C12">
         <v>0.04</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D12">
         <v>0.2</v>
       </c>
     </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13">
+        <v>0.12</v>
+      </c>
+      <c r="C13">
+        <v>0.02</v>
+      </c>
+      <c r="D13">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14">
+        <v>0.12</v>
+      </c>
+      <c r="C14">
+        <v>0.04</v>
+      </c>
+      <c r="D14">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>89</v>
+      </c>
+      <c r="B15">
+        <v>0.12</v>
+      </c>
+      <c r="C15">
+        <v>0.02</v>
+      </c>
+      <c r="D15">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>90</v>
+      </c>
+      <c r="B16">
+        <v>0.12</v>
+      </c>
+      <c r="C16">
+        <v>0.01</v>
+      </c>
+      <c r="D16">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>91</v>
+      </c>
+      <c r="B17">
+        <v>0.11</v>
+      </c>
+      <c r="C17">
+        <v>0.01</v>
+      </c>
+      <c r="D17">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18">
+        <v>0.11</v>
+      </c>
+      <c r="C18">
+        <v>0.02</v>
+      </c>
+      <c r="D18">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>93</v>
+      </c>
+      <c r="B19">
+        <v>0.11</v>
+      </c>
+      <c r="C19">
+        <v>0.02</v>
+      </c>
+      <c r="D19">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>94</v>
+      </c>
+      <c r="B20">
+        <v>0.11</v>
+      </c>
+      <c r="C20">
+        <v>0.02</v>
+      </c>
+      <c r="D20">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>95</v>
+      </c>
+      <c r="B21">
+        <v>0.1</v>
+      </c>
+      <c r="C21">
+        <v>0.02</v>
+      </c>
+      <c r="D21">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>96</v>
+      </c>
+      <c r="B22">
+        <v>0.09</v>
+      </c>
+      <c r="C22">
+        <v>0.02</v>
+      </c>
+      <c r="D22">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>97</v>
+      </c>
+      <c r="B23">
+        <v>0.09</v>
+      </c>
+      <c r="C23">
+        <v>0.02</v>
+      </c>
+      <c r="D23">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>98</v>
+      </c>
+      <c r="B24">
+        <v>0.08</v>
+      </c>
+      <c r="C24">
+        <v>0.03</v>
+      </c>
+      <c r="D24">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>99</v>
+      </c>
+      <c r="B25">
+        <v>0.08</v>
+      </c>
+      <c r="C25">
+        <v>0.02</v>
+      </c>
+      <c r="D25">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>100</v>
+      </c>
+      <c r="B26">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C26">
+        <v>0.01</v>
+      </c>
+      <c r="D26">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>101</v>
+      </c>
+      <c r="B27">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C27">
+        <v>0.01</v>
+      </c>
+      <c r="D27">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>102</v>
+      </c>
+      <c r="B28">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C28">
+        <v>0.02</v>
+      </c>
+      <c r="D28">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>103</v>
+      </c>
+      <c r="B29">
+        <v>0.06</v>
+      </c>
+      <c r="C29">
+        <v>0.01</v>
+      </c>
+      <c r="D29">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>104</v>
+      </c>
+      <c r="B30">
+        <v>0.06</v>
+      </c>
+      <c r="C30">
+        <v>0.01</v>
+      </c>
+      <c r="D30">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>105</v>
+      </c>
+      <c r="B31">
+        <v>0.06</v>
+      </c>
+      <c r="C31">
+        <v>0.01</v>
+      </c>
+      <c r="D31">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>106</v>
+      </c>
+      <c r="B32">
+        <v>0.05</v>
+      </c>
+      <c r="C32">
+        <v>0.01</v>
+      </c>
+      <c r="D32">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>107</v>
+      </c>
+      <c r="B33">
+        <v>0.05</v>
+      </c>
+      <c r="C33">
+        <v>0.01</v>
+      </c>
+      <c r="D33">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>108</v>
+      </c>
+      <c r="B34">
+        <v>0.05</v>
+      </c>
+      <c r="C34">
+        <v>0.02</v>
+      </c>
+      <c r="D34">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>109</v>
+      </c>
+      <c r="B35">
+        <v>0.05</v>
+      </c>
+      <c r="C35">
+        <v>0.01</v>
+      </c>
+      <c r="D35">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>110</v>
+      </c>
+      <c r="B36">
+        <v>0.04</v>
+      </c>
+      <c r="C36">
+        <v>0.01</v>
+      </c>
+      <c r="D36">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>111</v>
+      </c>
+      <c r="B37">
+        <v>0.03</v>
+      </c>
+      <c r="C37">
+        <v>0.01</v>
+      </c>
+      <c r="D37">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>112</v>
+      </c>
+      <c r="B38">
+        <v>0.03</v>
+      </c>
+      <c r="C38">
+        <v>0.01</v>
+      </c>
+      <c r="D38">
+        <v>0.09</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F59E4EC8-3E34-41D3-9315-A7C3365949FB}">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="14"/>
+      <c r="B2" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="10"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" s="14">
+        <v>2015</v>
+      </c>
+      <c r="C3" s="14">
+        <v>2017</v>
+      </c>
+      <c r="D3" s="14">
+        <v>2019</v>
+      </c>
+      <c r="E3" s="14">
+        <v>2020</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="G3" s="10"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="G4" s="10"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="G5" s="10"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="G6" s="10"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="G7" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B2:F2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>